<commit_message>
tweaked isolated voltage sensors
</commit_message>
<xml_diff>
--- a/MotorCalcs/motorware_selecting_user_variables.xlsx
+++ b/MotorCalcs/motorware_selecting_user_variables.xlsx
@@ -1064,7 +1064,7 @@
   <dimension ref="A1:J202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="I4" s="20">
         <f>ROUND(4*B13*0.95,0)</f>
-        <v>2090</v>
+        <v>2046</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>42</v>
@@ -1396,8 +1396,8 @@
         <v>35</v>
       </c>
       <c r="B13" s="4">
-        <f>1100/2</f>
-        <v>550</v>
+        <f>1/(2*PI()*10*10^-9*1/(1/30000+1/2000000))</f>
+        <v>538.4742241275793</v>
       </c>
       <c r="C13" s="29" t="s">
         <v>4</v>
@@ -1449,7 +1449,8 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>330</v>
+        <f>(30+2000)/30*(4.98*3.3/3.18)</f>
+        <v>349.69622641509437</v>
       </c>
       <c r="C15" s="29" t="s">
         <v>5</v>
@@ -1685,13 +1686,27 @@
       <c r="I26" s="46"/>
       <c r="J26" s="49"/>
     </row>
-    <row r="27" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="12">
+        <f>(30+2000)/30</f>
+        <v>67.666666666666671</v>
+      </c>
+    </row>
     <row r="28" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="F28" s="12">
+        <f>B15/F27</f>
+        <v>5.1679245283018869</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="12">
+        <f>F28*3.18/4.98</f>
+        <v>3.3</v>
+      </c>
+    </row>
     <row r="30" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I30" s="12">
         <f>300*0.15</f>

</xml_diff>